<commit_message>
Update the demo project
</commit_message>
<xml_diff>
--- a/demo_project/demo_metadata/metadata_demo.xlsx
+++ b/demo_project/demo_metadata/metadata_demo.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="161">
   <si>
     <t>sample_num</t>
   </si>
@@ -266,9 +266,6 @@
     <t>ph</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>After submission to SRA you can get these numbers.</t>
   </si>
   <si>
@@ -380,9 +377,6 @@
     <t>For all these SRA fields, only certain values are permitted.</t>
   </si>
   <si>
-    <t>aquatic metagenome</t>
-  </si>
-  <si>
     <t>For all these environemental SRA fields, only certain values are permitted.</t>
   </si>
   <si>
@@ -495,6 +489,27 @@
   </si>
   <si>
     <t>phred_threshold</t>
+  </si>
+  <si>
+    <t>sediment metagenome</t>
+  </si>
+  <si>
+    <t>SAMN08011025</t>
+  </si>
+  <si>
+    <t>SAMN04328859</t>
+  </si>
+  <si>
+    <t>marine sediment metagenome</t>
+  </si>
+  <si>
+    <t>SAMN10319704</t>
+  </si>
+  <si>
+    <t>biofilm metagenome</t>
+  </si>
+  <si>
+    <t>SAMN10320202</t>
   </si>
 </sst>
 </file>
@@ -921,7 +936,7 @@
   <dimension ref="A1:BW7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="BK1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="BX10" sqref="BX10"/>
+      <selection activeCell="BU12" sqref="BU12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1025,13 +1040,13 @@
         <v>18</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>25</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>17</v>
@@ -1049,7 +1064,7 @@
         <v>26</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>31</v>
@@ -1058,7 +1073,7 @@
         <v>32</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>39</v>
@@ -1079,19 +1094,19 @@
         <v>46</v>
       </c>
       <c r="AE1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AF1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AH1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>94</v>
       </c>
       <c r="AK1" s="1" t="s">
         <v>56</v>
@@ -1100,94 +1115,94 @@
         <v>57</v>
       </c>
       <c r="AN1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AO1" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AX1" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="AR1" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="AS1" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="AT1" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="AU1" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="AW1" s="1" t="s">
+      <c r="BB1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="BE1" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="BF1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="BG1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="BH1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="BI1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="BJ1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="BL1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="BN1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="BO1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="BP1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="BR1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="BS1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="BT1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="AX1" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="AY1" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="AZ1" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="BB1" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="BC1" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="BE1" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="BF1" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="BG1" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="BH1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="BI1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="BJ1" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="BL1" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="BN1" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="BO1" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="BP1" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="BR1" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="BS1" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="BT1" s="1" t="s">
+      <c r="BU1" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="BU1" s="1" t="s">
-        <v>114</v>
-      </c>
       <c r="BV1" s="9" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="BW1" s="9" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:75" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1210,10 +1225,10 @@
         <v>11</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>14</v>
@@ -1297,7 +1312,7 @@
         <v>62</v>
       </c>
       <c r="AQ2" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="AR2" s="2" t="s">
         <v>64</v>
@@ -1345,34 +1360,34 @@
         <v>78</v>
       </c>
       <c r="BL2" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="BN2" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="BO2" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="BO2" s="2" t="s">
-        <v>85</v>
-      </c>
       <c r="BP2" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="BR2" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="BS2" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="BT2" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="BU2" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="BU2" s="2" t="s">
-        <v>103</v>
-      </c>
       <c r="BV2" s="10" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="BW2" s="10" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:75" x14ac:dyDescent="0.2">
@@ -1383,34 +1398,31 @@
         <v>3</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F3" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="H3" s="4" t="s">
-        <v>131</v>
-      </c>
       <c r="I3" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="J3" s="4" t="s">
         <v>130</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>79</v>
       </c>
       <c r="N3" s="5">
         <v>22286</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="S3" s="4" t="s">
         <v>37</v>
@@ -1422,19 +1434,19 @@
         <v>36</v>
       </c>
       <c r="AE3" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="AF3" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="AG3" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="AF3" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="AG3" s="4" t="s">
-        <v>146</v>
-      </c>
       <c r="AH3" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="AI3" s="4" t="s">
         <v>143</v>
-      </c>
-      <c r="AI3" s="4" t="s">
-        <v>145</v>
       </c>
       <c r="AN3" s="4" t="s">
         <v>60</v>
@@ -1446,37 +1458,37 @@
         <v>63</v>
       </c>
       <c r="AQ3" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="AR3" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="AS3" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="AW3" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="BC3" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="BE3" s="8">
         <v>42704</v>
       </c>
       <c r="BL3" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="BR3" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BS3" s="4">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="BT3" s="4">
-        <v>200</v>
+        <v>2800</v>
       </c>
       <c r="BU3" s="4">
-        <v>350</v>
+        <v>5500</v>
       </c>
       <c r="BV3" s="4">
         <v>30</v>
@@ -1493,34 +1505,31 @@
         <v>3</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F4" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="H4" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="I4" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="J4" s="4" t="s">
         <v>131</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>79</v>
       </c>
       <c r="N4" s="5">
         <v>37850</v>
       </c>
       <c r="P4" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="S4" s="4" t="s">
         <v>37</v>
@@ -1532,19 +1541,19 @@
         <v>36</v>
       </c>
       <c r="AE4" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="AF4" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="AG4" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="AF4" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="AG4" s="4" t="s">
-        <v>146</v>
-      </c>
       <c r="AH4" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="AI4" s="4" t="s">
         <v>143</v>
-      </c>
-      <c r="AI4" s="4" t="s">
-        <v>145</v>
       </c>
       <c r="AN4" s="4" t="s">
         <v>60</v>
@@ -1556,34 +1565,37 @@
         <v>63</v>
       </c>
       <c r="AQ4" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="AR4" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="AS4" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="AW4" s="4" t="s">
-        <v>117</v>
+        <v>154</v>
+      </c>
+      <c r="BC4" s="4" t="s">
+        <v>155</v>
       </c>
       <c r="BE4" s="8">
-        <v>44012</v>
+        <v>41487</v>
       </c>
       <c r="BL4" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="BR4" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BS4" s="4">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="BT4" s="4">
-        <v>200</v>
+        <v>2800</v>
       </c>
       <c r="BU4" s="4">
-        <v>350</v>
+        <v>5500</v>
       </c>
       <c r="BV4" s="4">
         <v>30</v>
@@ -1600,34 +1612,31 @@
         <v>3</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F5" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="H5" s="4" t="s">
-        <v>131</v>
-      </c>
       <c r="I5" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>79</v>
+        <v>132</v>
       </c>
       <c r="N5" s="5">
         <v>28549</v>
       </c>
       <c r="P5" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="S5" s="4" t="s">
         <v>37</v>
@@ -1639,19 +1648,19 @@
         <v>36</v>
       </c>
       <c r="AE5" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="AF5" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="AG5" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="AF5" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="AG5" s="4" t="s">
-        <v>146</v>
-      </c>
       <c r="AH5" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="AI5" s="4" t="s">
         <v>143</v>
-      </c>
-      <c r="AI5" s="4" t="s">
-        <v>145</v>
       </c>
       <c r="AN5" s="4" t="s">
         <v>60</v>
@@ -1663,34 +1672,37 @@
         <v>63</v>
       </c>
       <c r="AQ5" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="AR5" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="AS5" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="AW5" s="4" t="s">
-        <v>117</v>
+        <v>157</v>
+      </c>
+      <c r="BC5" s="4" t="s">
+        <v>156</v>
       </c>
       <c r="BE5" s="8">
-        <v>44012</v>
+        <v>41395</v>
       </c>
       <c r="BL5" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="BR5" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BS5" s="4">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="BT5" s="4">
-        <v>200</v>
+        <v>2800</v>
       </c>
       <c r="BU5" s="4">
-        <v>350</v>
+        <v>5500</v>
       </c>
       <c r="BV5" s="4">
         <v>30</v>
@@ -1707,34 +1719,31 @@
         <v>3</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E6" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="H6" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="H6" s="4" t="s">
-        <v>131</v>
-      </c>
       <c r="I6" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>79</v>
+        <v>133</v>
       </c>
       <c r="N6" s="5">
         <v>22972</v>
       </c>
       <c r="P6" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="S6" s="4" t="s">
         <v>37</v>
@@ -1746,19 +1755,19 @@
         <v>36</v>
       </c>
       <c r="AE6" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="AF6" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="AG6" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="AF6" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="AG6" s="4" t="s">
-        <v>146</v>
-      </c>
       <c r="AH6" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="AI6" s="4" t="s">
         <v>143</v>
-      </c>
-      <c r="AI6" s="4" t="s">
-        <v>145</v>
       </c>
       <c r="AN6" s="4" t="s">
         <v>60</v>
@@ -1770,34 +1779,37 @@
         <v>63</v>
       </c>
       <c r="AQ6" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="AR6" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="AS6" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="AW6" s="4" t="s">
-        <v>117</v>
+        <v>159</v>
+      </c>
+      <c r="BC6" s="4" t="s">
+        <v>158</v>
       </c>
       <c r="BE6" s="8">
-        <v>44012</v>
+        <v>43972</v>
       </c>
       <c r="BL6" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="BR6" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BS6" s="4">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="BT6" s="4">
-        <v>200</v>
+        <v>2800</v>
       </c>
       <c r="BU6" s="4">
-        <v>350</v>
+        <v>5500</v>
       </c>
       <c r="BV6" s="4">
         <v>30</v>
@@ -1814,34 +1826,31 @@
         <v>3</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="I7" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="F7" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>130</v>
-      </c>
       <c r="J7" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>79</v>
+        <v>134</v>
       </c>
       <c r="N7" s="5">
         <v>25253</v>
       </c>
       <c r="P7" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="S7" s="4" t="s">
         <v>37</v>
@@ -1853,19 +1862,19 @@
         <v>36</v>
       </c>
       <c r="AE7" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="AF7" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="AG7" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="AF7" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="AG7" s="4" t="s">
-        <v>146</v>
-      </c>
       <c r="AH7" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="AI7" s="4" t="s">
         <v>143</v>
-      </c>
-      <c r="AI7" s="4" t="s">
-        <v>145</v>
       </c>
       <c r="AN7" s="4" t="s">
         <v>60</v>
@@ -1877,34 +1886,37 @@
         <v>63</v>
       </c>
       <c r="AQ7" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="AR7" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="AS7" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="AW7" s="4" t="s">
-        <v>117</v>
+        <v>157</v>
+      </c>
+      <c r="BC7" s="4" t="s">
+        <v>160</v>
       </c>
       <c r="BE7" s="8">
-        <v>44012</v>
+        <v>38869</v>
       </c>
       <c r="BL7" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="BR7" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BS7" s="4">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="BT7" s="4">
-        <v>200</v>
+        <v>2800</v>
       </c>
       <c r="BU7" s="4">
-        <v>350</v>
+        <v>5500</v>
       </c>
       <c r="BV7" s="4">
         <v>30</v>

</xml_diff>

<commit_message>
Customizing the rank levels of Project reports
</commit_message>
<xml_diff>
--- a/demo_project/demo_metadata/metadata_demo.xlsx
+++ b/demo_project/demo_metadata/metadata_demo.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="164">
   <si>
     <t>sample_num</t>
   </si>
@@ -510,6 +510,15 @@
   </si>
   <si>
     <t>SAMN10320202</t>
+  </si>
+  <si>
+    <t>taxa_barstacks</t>
+  </si>
+  <si>
+    <t>phylum, class</t>
+  </si>
+  <si>
+    <t>This property determines how many taxonomical barstacks plots are included in the project report. Seperate each value with a comma. Possible values are: "phylum, class, order, family, genus, species"</t>
   </si>
 </sst>
 </file>
@@ -933,10 +942,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BW7"/>
+  <dimension ref="A1:BY7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BK1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="BU12" sqref="BU12"/>
+    <sheetView tabSelected="1" topLeftCell="BL1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="BU17" sqref="BU17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1014,10 +1023,12 @@
     <col min="73" max="73" width="20.83203125" style="4" customWidth="1"/>
     <col min="74" max="74" width="21.83203125" style="4" customWidth="1"/>
     <col min="75" max="75" width="22.6640625" style="4" customWidth="1"/>
-    <col min="76" max="16384" width="10.83203125" style="4"/>
+    <col min="76" max="76" width="10.83203125" style="4"/>
+    <col min="77" max="77" width="24.5" style="4" customWidth="1"/>
+    <col min="78" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:75" s="1" customFormat="1" ht="154" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:77" s="1" customFormat="1" ht="154" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -1204,8 +1215,11 @@
       <c r="BW1" s="9" t="s">
         <v>151</v>
       </c>
+      <c r="BY1" s="1" t="s">
+        <v>163</v>
+      </c>
     </row>
-    <row r="2" spans="1:75" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:77" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1389,8 +1403,11 @@
       <c r="BW2" s="10" t="s">
         <v>153</v>
       </c>
+      <c r="BY2" s="2" t="s">
+        <v>161</v>
+      </c>
     </row>
-    <row r="3" spans="1:75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -1496,8 +1513,11 @@
       <c r="BW3" s="4">
         <v>20</v>
       </c>
+      <c r="BY3" s="4" t="s">
+        <v>162</v>
+      </c>
     </row>
-    <row r="4" spans="1:75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -1603,8 +1623,11 @@
       <c r="BW4" s="4">
         <v>20</v>
       </c>
+      <c r="BY4" s="4" t="s">
+        <v>162</v>
+      </c>
     </row>
-    <row r="5" spans="1:75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -1710,8 +1733,11 @@
       <c r="BW5" s="4">
         <v>20</v>
       </c>
+      <c r="BY5" s="4" t="s">
+        <v>162</v>
+      </c>
     </row>
-    <row r="6" spans="1:75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -1817,8 +1843,11 @@
       <c r="BW6" s="4">
         <v>20</v>
       </c>
+      <c r="BY6" s="4" t="s">
+        <v>162</v>
+      </c>
     </row>
-    <row r="7" spans="1:75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -1923,6 +1952,9 @@
       </c>
       <c r="BW7" s="4">
         <v>20</v>
+      </c>
+      <c r="BY7" s="4" t="s">
+        <v>162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixing the overflowing legend of taxa tables in Project reports
</commit_message>
<xml_diff>
--- a/demo_project/demo_metadata/metadata_demo.xlsx
+++ b/demo_project/demo_metadata/metadata_demo.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="166">
   <si>
     <t>sample_num</t>
   </si>
@@ -519,6 +519,12 @@
   </si>
   <si>
     <t>This property determines how many taxonomical barstacks plots are included in the project report. Seperate each value with a comma. Possible values are: "phylum, class, order, family, genus, species"</t>
+  </si>
+  <si>
+    <t>max_taxa</t>
+  </si>
+  <si>
+    <t>This determines how many taxaonmic names will be displayed in each graph at a maximum. Remaining entries are combined into 'others'.</t>
   </si>
 </sst>
 </file>
@@ -942,10 +948,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BY7"/>
+  <dimension ref="A1:BZ7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="BL1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="BU17" sqref="BU17"/>
+      <selection activeCell="BZ17" sqref="BZ17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1025,10 +1031,11 @@
     <col min="75" max="75" width="22.6640625" style="4" customWidth="1"/>
     <col min="76" max="76" width="10.83203125" style="4"/>
     <col min="77" max="77" width="24.5" style="4" customWidth="1"/>
-    <col min="78" max="16384" width="10.83203125" style="4"/>
+    <col min="78" max="78" width="18.1640625" style="4" customWidth="1"/>
+    <col min="79" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:77" s="1" customFormat="1" ht="154" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:78" s="1" customFormat="1" ht="154" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -1218,8 +1225,11 @@
       <c r="BY1" s="1" t="s">
         <v>163</v>
       </c>
+      <c r="BZ1" s="1" t="s">
+        <v>165</v>
+      </c>
     </row>
-    <row r="2" spans="1:77" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:78" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1406,8 +1416,11 @@
       <c r="BY2" s="2" t="s">
         <v>161</v>
       </c>
+      <c r="BZ2" s="2" t="s">
+        <v>164</v>
+      </c>
     </row>
-    <row r="3" spans="1:77" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:78" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -1516,8 +1529,11 @@
       <c r="BY3" s="4" t="s">
         <v>162</v>
       </c>
+      <c r="BZ3" s="4">
+        <v>18</v>
+      </c>
     </row>
-    <row r="4" spans="1:77" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:78" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -1626,8 +1642,11 @@
       <c r="BY4" s="4" t="s">
         <v>162</v>
       </c>
+      <c r="BZ4" s="4">
+        <v>18</v>
+      </c>
     </row>
-    <row r="5" spans="1:77" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:78" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -1736,8 +1755,11 @@
       <c r="BY5" s="4" t="s">
         <v>162</v>
       </c>
+      <c r="BZ5" s="4">
+        <v>18</v>
+      </c>
     </row>
-    <row r="6" spans="1:77" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:78" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -1846,8 +1868,11 @@
       <c r="BY6" s="4" t="s">
         <v>162</v>
       </c>
+      <c r="BZ6" s="4">
+        <v>18</v>
+      </c>
     </row>
-    <row r="7" spans="1:77" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:78" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -1955,6 +1980,9 @@
       </c>
       <c r="BY7" s="4" t="s">
         <v>162</v>
+      </c>
+      <c r="BZ7" s="4">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add an optional column to the metadata file: barrnap_mode
</commit_message>
<xml_diff>
--- a/demo_project/demo_metadata/metadata_demo.xlsx
+++ b/demo_project/demo_metadata/metadata_demo.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="169">
   <si>
     <t>sample_num</t>
   </si>
@@ -525,6 +525,15 @@
   </si>
   <si>
     <t>This determines how many taxaonmic names will be displayed in each graph at a maximum. Remaining entries are combined into 'others'.</t>
+  </si>
+  <si>
+    <t>barrnap_mode</t>
+  </si>
+  <si>
+    <t>on</t>
+  </si>
+  <si>
+    <t>Should barrnap be run on the sample to detect the presence of rRNA genes? This value can be either "on" or "off". This column is optional.</t>
   </si>
 </sst>
 </file>
@@ -534,7 +543,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -587,6 +596,12 @@
       <b/>
       <sz val="12"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Menlo"/>
       <family val="2"/>
     </font>
@@ -643,7 +658,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -669,6 +684,7 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -948,10 +964,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BZ7"/>
+  <dimension ref="A1:CA7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="BL1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="AF18" sqref="AF18"/>
+      <selection activeCell="BX1" sqref="BX1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1028,14 +1044,14 @@
     <col min="72" max="72" width="19.33203125" style="4" customWidth="1"/>
     <col min="73" max="73" width="20.83203125" style="4" customWidth="1"/>
     <col min="74" max="74" width="21.83203125" style="4" customWidth="1"/>
-    <col min="75" max="75" width="22.6640625" style="4" customWidth="1"/>
-    <col min="76" max="76" width="10.83203125" style="4"/>
-    <col min="77" max="77" width="24.5" style="4" customWidth="1"/>
-    <col min="78" max="78" width="18.1640625" style="4" customWidth="1"/>
-    <col min="79" max="16384" width="10.83203125" style="4"/>
+    <col min="75" max="76" width="22.6640625" style="4" customWidth="1"/>
+    <col min="77" max="77" width="10.83203125" style="4"/>
+    <col min="78" max="78" width="24.5" style="4" customWidth="1"/>
+    <col min="79" max="79" width="18.1640625" style="4" customWidth="1"/>
+    <col min="80" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:78" s="1" customFormat="1" ht="154" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:79" s="1" customFormat="1" ht="154" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -1222,14 +1238,17 @@
       <c r="BW1" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="BY1" s="1" t="s">
+      <c r="BX1" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="BZ1" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="BZ1" s="1" t="s">
+      <c r="CA1" s="1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:78" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:79" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1413,14 +1432,17 @@
       <c r="BW2" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="BY2" s="2" t="s">
+      <c r="BX2" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="BZ2" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="BZ2" s="2" t="s">
+      <c r="CA2" s="2" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="3" spans="1:78" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -1526,14 +1548,17 @@
       <c r="BW3" s="4">
         <v>20</v>
       </c>
-      <c r="BY3" s="4" t="s">
+      <c r="BX3" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="BZ3" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="BZ3" s="4">
+      <c r="CA3" s="4">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:78" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -1639,14 +1664,17 @@
       <c r="BW4" s="4">
         <v>20</v>
       </c>
-      <c r="BY4" s="4" t="s">
+      <c r="BX4" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="BZ4" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="BZ4" s="4">
+      <c r="CA4" s="4">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:78" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -1752,14 +1780,17 @@
       <c r="BW5" s="4">
         <v>20</v>
       </c>
-      <c r="BY5" s="4" t="s">
+      <c r="BX5" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="BZ5" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="BZ5" s="4">
+      <c r="CA5" s="4">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:78" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -1865,14 +1896,17 @@
       <c r="BW6" s="4">
         <v>20</v>
       </c>
-      <c r="BY6" s="4" t="s">
+      <c r="BX6" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="BZ6" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="BZ6" s="4">
+      <c r="CA6" s="4">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:78" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -1978,10 +2012,13 @@
       <c r="BW7" s="4">
         <v>20</v>
       </c>
-      <c r="BY7" s="4" t="s">
+      <c r="BX7" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="BZ7" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="BZ7" s="4">
+      <c r="CA7" s="4">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added 4 barrnap modes customizable via excel
</commit_message>
<xml_diff>
--- a/demo_project/demo_metadata/metadata_demo.xlsx
+++ b/demo_project/demo_metadata/metadata_demo.xlsx
@@ -530,10 +530,15 @@
     <t>barrnap_mode</t>
   </si>
   <si>
-    <t>on</t>
-  </si>
-  <si>
-    <t>Should barrnap be run on the sample to detect the presence of rRNA genes? This value can be either "on" or "off". This column is optional.</t>
+    <t>trim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Should barrnap be run on the sample to detect the presence of rRNA genes? This column is optional. This value can be:
+      - "off": Will skip gene detection (default). 
+      - "filter": To remove reads that didn't have hits for both 16S and 23S.
+      - "concat": To remove the ITS region between 16S and 23S.
+      - "trim": To remove the 23S and keep the 16S portion only of every read.
+</t>
   </si>
 </sst>
 </file>
@@ -967,7 +972,7 @@
   <dimension ref="A1:CA7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="BL1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="BX1" sqref="BX1"/>
+      <selection activeCell="BX9" sqref="BX9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1044,7 +1049,8 @@
     <col min="72" max="72" width="19.33203125" style="4" customWidth="1"/>
     <col min="73" max="73" width="20.83203125" style="4" customWidth="1"/>
     <col min="74" max="74" width="21.83203125" style="4" customWidth="1"/>
-    <col min="75" max="76" width="22.6640625" style="4" customWidth="1"/>
+    <col min="75" max="75" width="22.6640625" style="4" customWidth="1"/>
+    <col min="76" max="76" width="38.83203125" style="4" customWidth="1"/>
     <col min="77" max="77" width="10.83203125" style="4"/>
     <col min="78" max="78" width="24.5" style="4" customWidth="1"/>
     <col min="79" max="79" width="18.1640625" style="4" customWidth="1"/>

</xml_diff>

<commit_message>
Add barrnap mode to excel file
</commit_message>
<xml_diff>
--- a/demo_project/demo_metadata/metadata_demo.xlsx
+++ b/demo_project/demo_metadata/metadata_demo.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="40" yWindow="1740" windowWidth="51120" windowHeight="28340" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51120" windowHeight="28340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="175">
   <si>
     <t>sample_num</t>
   </si>
@@ -545,6 +545,18 @@
   </si>
   <si>
     <t>instrument_software</t>
+  </si>
+  <si>
+    <t>otu_threshold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This will determine the percentage of similarty that two sequences must share for them to be clustered into the same OTU. This is an optional column with a default value of 0.97 </t>
+  </si>
+  <si>
+    <t>otu_min_size</t>
+  </si>
+  <si>
+    <t>This will determine the minimum size of an OTU. Below this size OTUs are discarded. This is an optional column with a default value of 1. Setting this value to 2 will remove all singeltons for instance.</t>
   </si>
 </sst>
 </file>
@@ -979,10 +991,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CB7"/>
+  <dimension ref="A1:CE7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="BP1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="AV8" sqref="AV8"/>
+      <selection activeCell="BZ17" sqref="BZ17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1059,15 +1071,15 @@
     <col min="73" max="73" width="19.33203125" style="4" customWidth="1"/>
     <col min="74" max="74" width="20.83203125" style="4" customWidth="1"/>
     <col min="75" max="75" width="21.83203125" style="4" customWidth="1"/>
-    <col min="76" max="76" width="22.6640625" style="4" customWidth="1"/>
-    <col min="77" max="77" width="38.83203125" style="4" customWidth="1"/>
-    <col min="78" max="78" width="10.83203125" style="4"/>
-    <col min="79" max="79" width="24.5" style="4" customWidth="1"/>
-    <col min="80" max="80" width="18.1640625" style="4" customWidth="1"/>
-    <col min="81" max="16384" width="10.83203125" style="4"/>
+    <col min="76" max="79" width="22.6640625" style="4" customWidth="1"/>
+    <col min="80" max="80" width="38.83203125" style="4" customWidth="1"/>
+    <col min="81" max="81" width="10.83203125" style="4"/>
+    <col min="82" max="82" width="24.5" style="4" customWidth="1"/>
+    <col min="83" max="83" width="18.1640625" style="4" customWidth="1"/>
+    <col min="84" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:80" s="1" customFormat="1" ht="154" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:83" s="1" customFormat="1" ht="154" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -1257,17 +1269,24 @@
       <c r="BX1" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="BY1" s="9" t="s">
+      <c r="BY1" s="9"/>
+      <c r="BZ1" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="CA1" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="CB1" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="CA1" s="1" t="s">
+      <c r="CD1" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="CB1" s="1" t="s">
+      <c r="CE1" s="1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:80" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:83" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1454,17 +1473,24 @@
       <c r="BX2" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="BY2" s="10" t="s">
+      <c r="BY2" s="10"/>
+      <c r="BZ2" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="CA2" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="CB2" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="CA2" s="2" t="s">
+      <c r="CD2" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="CB2" s="2" t="s">
+      <c r="CE2" s="2" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="3" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:83" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -1570,17 +1596,23 @@
       <c r="BX3" s="4">
         <v>20</v>
       </c>
-      <c r="BY3" s="11" t="s">
+      <c r="BZ3" s="4">
+        <v>0.97</v>
+      </c>
+      <c r="CA3" s="4">
+        <v>2</v>
+      </c>
+      <c r="CB3" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="CA3" s="4" t="s">
+      <c r="CD3" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="CB3" s="4">
+      <c r="CE3" s="4">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:83" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -1686,17 +1718,23 @@
       <c r="BX4" s="4">
         <v>20</v>
       </c>
-      <c r="BY4" s="11" t="s">
+      <c r="BZ4" s="4">
+        <v>0.97</v>
+      </c>
+      <c r="CA4" s="4">
+        <v>2</v>
+      </c>
+      <c r="CB4" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="CA4" s="4" t="s">
+      <c r="CD4" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="CB4" s="4">
+      <c r="CE4" s="4">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:83" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -1802,17 +1840,23 @@
       <c r="BX5" s="4">
         <v>20</v>
       </c>
-      <c r="BY5" s="11" t="s">
+      <c r="BZ5" s="4">
+        <v>0.97</v>
+      </c>
+      <c r="CA5" s="4">
+        <v>2</v>
+      </c>
+      <c r="CB5" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="CA5" s="4" t="s">
+      <c r="CD5" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="CB5" s="4">
+      <c r="CE5" s="4">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:83" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -1918,17 +1962,23 @@
       <c r="BX6" s="4">
         <v>20</v>
       </c>
-      <c r="BY6" s="11" t="s">
+      <c r="BZ6" s="4">
+        <v>0.97</v>
+      </c>
+      <c r="CA6" s="4">
+        <v>2</v>
+      </c>
+      <c r="CB6" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="CA6" s="4" t="s">
+      <c r="CD6" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="CB6" s="4">
+      <c r="CE6" s="4">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:83" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -2034,13 +2084,19 @@
       <c r="BX7" s="4">
         <v>20</v>
       </c>
-      <c r="BY7" s="11" t="s">
+      <c r="BZ7" s="4">
+        <v>0.97</v>
+      </c>
+      <c r="CA7" s="4">
+        <v>2</v>
+      </c>
+      <c r="CB7" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="CA7" s="4" t="s">
+      <c r="CD7" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="CB7" s="4">
+      <c r="CE7" s="4">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add method to dereplicate the vsearch results
</commit_message>
<xml_diff>
--- a/demo_project/demo_metadata/metadata_demo.xlsx
+++ b/demo_project/demo_metadata/metadata_demo.xlsx
@@ -556,7 +556,7 @@
     <t>otu_min_size</t>
   </si>
   <si>
-    <t>This will determine the minimum size of an OTU. Below this size OTUs are discarded. This is an optional column with a default value of 1. Setting this value to 2 will remove all singeltons for instance.</t>
+    <t>This will determine the minimum size of an OTU. Below this size OTUs are discarded. This is an optional column with a default value of 1. For instance, setting this value to 2 will remove all singeltons.</t>
   </si>
 </sst>
 </file>
@@ -993,8 +993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CE7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BP1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="BZ17" sqref="BZ17"/>
+    <sheetView tabSelected="1" topLeftCell="BT1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="CB28" sqref="CB28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Set the demo project to trim mode and otu size 2
</commit_message>
<xml_diff>
--- a/demo_project/demo_metadata/metadata_demo.xlsx
+++ b/demo_project/demo_metadata/metadata_demo.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10913"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sinclair/repos/pacmill/demo_project/demo_metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D4408BE-7445-9142-9EC2-54E587F396D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51120" windowHeight="28340" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -530,9 +531,6 @@
     <t>barrnap_mode</t>
   </si>
   <si>
-    <t>trim</t>
-  </si>
-  <si>
     <t xml:space="preserve">Should barrnap be run on the sample to detect the presence of rRNA genes? This column is optional. This value can be:
      - "off": Will skip gene detection (default). 
      - "filter": To remove reads that didn't have hits for both 16S and 23S.
@@ -561,11 +559,14 @@
   <si>
     <t>~/output/demo_project/</t>
   </si>
+  <si>
+    <t>concat</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
@@ -726,6 +727,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -993,11 +997,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CE7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BC1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="BM12" sqref="BM12"/>
+    <sheetView tabSelected="1" topLeftCell="BV1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="CA13" sqref="CA13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1198,7 +1202,7 @@
         <v>115</v>
       </c>
       <c r="AT1" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="AU1" s="1" t="s">
         <v>109</v>
@@ -1274,13 +1278,13 @@
       </c>
       <c r="BY1" s="9"/>
       <c r="BZ1" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="CA1" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="CB1" s="9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="CD1" s="1" t="s">
         <v>163</v>
@@ -1405,7 +1409,7 @@
         <v>65</v>
       </c>
       <c r="AT2" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="AU2" s="2" t="s">
         <v>66</v>
@@ -1478,10 +1482,10 @@
       </c>
       <c r="BY2" s="10"/>
       <c r="BZ2" s="10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="CA2" s="10" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="CB2" s="10" t="s">
         <v>166</v>
@@ -1579,7 +1583,7 @@
         <v>42704</v>
       </c>
       <c r="BM3" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="BS3" s="4">
         <v>2</v>
@@ -1603,10 +1607,10 @@
         <v>0.97</v>
       </c>
       <c r="CA3" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="CB3" s="11" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="CD3" s="4" t="s">
         <v>162</v>
@@ -1701,7 +1705,7 @@
         <v>41487</v>
       </c>
       <c r="BM4" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="BS4" s="4">
         <v>2</v>
@@ -1725,10 +1729,10 @@
         <v>0.97</v>
       </c>
       <c r="CA4" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="CB4" s="11" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="CD4" s="4" t="s">
         <v>162</v>
@@ -1823,7 +1827,7 @@
         <v>41395</v>
       </c>
       <c r="BM5" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="BS5" s="4">
         <v>2</v>
@@ -1847,10 +1851,10 @@
         <v>0.97</v>
       </c>
       <c r="CA5" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="CB5" s="11" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="CD5" s="4" t="s">
         <v>162</v>
@@ -1945,7 +1949,7 @@
         <v>43972</v>
       </c>
       <c r="BM6" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="BS6" s="4">
         <v>2</v>
@@ -1969,10 +1973,10 @@
         <v>0.97</v>
       </c>
       <c r="CA6" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="CB6" s="11" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="CD6" s="4" t="s">
         <v>162</v>
@@ -2067,7 +2071,7 @@
         <v>38869</v>
       </c>
       <c r="BM7" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="BS7" s="4">
         <v>2</v>
@@ -2091,10 +2095,10 @@
         <v>0.97</v>
       </c>
       <c r="CA7" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="CB7" s="11" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="CD7" s="4" t="s">
         <v>162</v>

</xml_diff>

<commit_message>
Add an option to individually switch on/off taxonomic classification algorithms
</commit_message>
<xml_diff>
--- a/demo_project/demo_metadata/metadata_demo.xlsx
+++ b/demo_project/demo_metadata/metadata_demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sinclair/repos/pacmill/demo_project/demo_metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D4408BE-7445-9142-9EC2-54E587F396D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EBEB6F8-602B-0C42-B5F1-BD973FC123E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="440" windowWidth="37540" windowHeight="24440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="186">
   <si>
     <t>sample_num</t>
   </si>
@@ -561,6 +561,36 @@
   </si>
   <si>
     <t>concat</t>
+  </si>
+  <si>
+    <t>run_silva</t>
+  </si>
+  <si>
+    <t>run_greengenes</t>
+  </si>
+  <si>
+    <t>run_rdp</t>
+  </si>
+  <si>
+    <t>run_crest</t>
+  </si>
+  <si>
+    <t>run_ncbi_blast</t>
+  </si>
+  <si>
+    <t>When this option is turned on, we will run the Silva taxonomic classification and produce a report. This option can be set to "TRUE" or to "FALSE".</t>
+  </si>
+  <si>
+    <t>When this option is turned on, we will run the Green Genes taxonomic classification and produce a report. This option can be set to "TRUE" or to "FALSE".</t>
+  </si>
+  <si>
+    <t>When this option is turned on, we will run the RDP taxonomic classification and produce a report. This option can be set to "TRUE" or to "FALSE".</t>
+  </si>
+  <si>
+    <t>When this option is turned on, we will run the NCBI BLAST taxonomic classification and produce a report. This option can be set to "TRUE" or to "FALSE".</t>
+  </si>
+  <si>
+    <t>When this option is turned on, we will run the CREST LCA taxonomic classification and produce a report. This option can be set to "TRUE" or to "FALSE".</t>
   </si>
 </sst>
 </file>
@@ -998,10 +1028,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CE7"/>
+  <dimension ref="A1:CK7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BV1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="CA13" sqref="CA13"/>
+    <sheetView tabSelected="1" topLeftCell="CB1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="CF11" sqref="CF11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1081,12 +1111,18 @@
     <col min="76" max="79" width="22.6640625" style="4" customWidth="1"/>
     <col min="80" max="80" width="38.83203125" style="4" customWidth="1"/>
     <col min="81" max="81" width="10.83203125" style="4"/>
-    <col min="82" max="82" width="24.5" style="4" customWidth="1"/>
-    <col min="83" max="83" width="18.1640625" style="4" customWidth="1"/>
-    <col min="84" max="16384" width="10.83203125" style="4"/>
+    <col min="82" max="82" width="18.5" style="4" customWidth="1"/>
+    <col min="83" max="83" width="19" style="4" customWidth="1"/>
+    <col min="84" max="84" width="18.5" style="4" customWidth="1"/>
+    <col min="85" max="85" width="18.83203125" style="4" customWidth="1"/>
+    <col min="86" max="86" width="20.33203125" style="4" customWidth="1"/>
+    <col min="87" max="87" width="10.83203125" style="4"/>
+    <col min="88" max="88" width="24.5" style="4" customWidth="1"/>
+    <col min="89" max="89" width="18.1640625" style="4" customWidth="1"/>
+    <col min="90" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:83" s="1" customFormat="1" ht="154" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:89" s="1" customFormat="1" ht="154" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -1287,13 +1323,28 @@
         <v>167</v>
       </c>
       <c r="CD1" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="CE1" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="CF1" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="CG1" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="CH1" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="CJ1" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="CE1" s="1" t="s">
+      <c r="CK1" s="1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:83" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:89" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1491,13 +1542,28 @@
         <v>166</v>
       </c>
       <c r="CD2" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="CE2" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="CF2" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="CG2" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="CH2" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="CJ2" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="CE2" s="2" t="s">
+      <c r="CK2" s="2" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="3" spans="1:83" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:89" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -1612,14 +1678,29 @@
       <c r="CB3" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="CD3" s="4" t="s">
+      <c r="CD3" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="CE3" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="CF3" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="CG3" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="CH3" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="CJ3" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="CE3" s="4">
+      <c r="CK3" s="4">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:83" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:89" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -1734,14 +1815,29 @@
       <c r="CB4" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="CD4" s="4" t="s">
+      <c r="CD4" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="CE4" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="CF4" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="CG4" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="CH4" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="CJ4" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="CE4" s="4">
+      <c r="CK4" s="4">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:83" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:89" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -1856,14 +1952,29 @@
       <c r="CB5" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="CD5" s="4" t="s">
+      <c r="CD5" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="CE5" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="CF5" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="CG5" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="CH5" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="CJ5" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="CE5" s="4">
+      <c r="CK5" s="4">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:83" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:89" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -1978,14 +2089,29 @@
       <c r="CB6" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="CD6" s="4" t="s">
+      <c r="CD6" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="CE6" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="CF6" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="CG6" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="CH6" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="CJ6" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="CE6" s="4">
+      <c r="CK6" s="4">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:83" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:89" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -2100,10 +2226,25 @@
       <c r="CB7" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="CD7" s="4" t="s">
+      <c r="CD7" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="CE7" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="CF7" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="CG7" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="CH7" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="CJ7" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="CE7" s="4">
+      <c r="CK7" s="4">
         <v>18</v>
       </c>
     </row>

</xml_diff>